<commit_message>
feat: add laporan MarkDown
</commit_message>
<xml_diff>
--- a/Load Testing Result.xlsx
+++ b/Load Testing Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\9_Alfa\2_Materi Kuliah\Informatika\Semester5\JARKOM\Praktikum 3_Jarkom_F01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E39782E-F003-496A-9310-21527D992A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B33C401-CABA-4954-AFE7-569DC0737496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{C75504EF-4640-4AE8-9B88-BF4FA95FA6B6}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C75504EF-4640-4AE8-9B88-BF4FA95FA6B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Test Result" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -688,7 +688,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -700,6 +700,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Round Robin T</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1184,7 +1209,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1195,37 +1220,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3528,7 +3523,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3908,9 +3903,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3920,7 +3916,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4051,7 +4047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D66838-5579-4618-A4D2-D4E5543C89EB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4083,9 +4079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2071FB85-3468-4AE6-B9C8-301FDFB2B627}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>